<commit_message>
Solucion bugs y boton reactivar periodo
Se solucoinan bugs que presentaba el sistema:
Error al genrar caratula de pago y layout.
Se corrige detalle en reportes (En observaciónes mostraba información erronea)
Se agrega boton para que administradores puedan re abrir periodo de pago (Caeratula)
</commit_message>
<xml_diff>
--- a/winAsimilados/Resources/Formato_Masivo_Clientes.xlsx
+++ b/winAsimilados/Resources/Formato_Masivo_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aespejel\source\repos\winAsimilados\winAsimilados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F632F01A-207B-430E-816E-C6564DBE7452}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F463A1-3640-41B4-B860-FD58260B1056}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9A0A8DAE-14D7-40C1-AFA8-DE8507705D67}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>CLIENTE</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>COMISIONISTA 3</t>
-  </si>
-  <si>
-    <t>COMISIONISTA 4</t>
   </si>
 </sst>
 </file>
@@ -496,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16AEB8DF-E05E-4A23-BE8A-17EB7242BF2B}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,29 +505,29 @@
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="35" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="35" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -556,76 +553,70 @@
         <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -638,43 +629,43 @@
       <c r="D2">
         <v>100</v>
       </c>
+      <c r="I2">
+        <v>0.02</v>
+      </c>
+      <c r="J2">
+        <v>0.08</v>
+      </c>
       <c r="K2">
-        <v>0.02</v>
-      </c>
-      <c r="L2">
-        <v>0.08</v>
-      </c>
-      <c r="M2">
         <v>0.1</v>
       </c>
-      <c r="N2" t="s">
+      <c r="L2" t="s">
         <v>9</v>
       </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2">
+        <v>0.06</v>
+      </c>
       <c r="O2" t="s">
-        <v>9</v>
-      </c>
-      <c r="P2">
-        <v>0.06</v>
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>11</v>
       </c>
       <c r="Q2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="S2" t="s">
-        <v>12</v>
-      </c>
-      <c r="T2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U2" t="s">
         <v>14</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AA2" t="s">
         <v>15</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>